<commit_message>
PEM, Alkaline and SOEC Electrolyzer efficiencies
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc.eco\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc.eco\Documents\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D04F7D4A-5AA1-49C7-B56F-B175AF9AC679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09A41BD-41AF-4A9C-BCBB-49783ABECEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency_PEM" sheetId="5" r:id="rId1"/>
     <sheet name="Efficiency_Alkaline" sheetId="6" r:id="rId2"/>
-    <sheet name="Sources" sheetId="2" r:id="rId3"/>
+    <sheet name="Efficiency_SOEC" sheetId="7" r:id="rId3"/>
+    <sheet name="Sources" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Power [%]</t>
   </si>
@@ -56,6 +57,18 @@
   </si>
   <si>
     <t>Sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOEC: </t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9025002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and for the max efficiency: </t>
+  </si>
+  <si>
+    <t>https://www.sunfire.de/files/sunfire/images/content/Produkte_Technologie/factsheets/Sunfire-Factsheet-HyLink-SOEC_2023Nov.pdf</t>
   </si>
 </sst>
 </file>
@@ -614,14 +627,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -659,7 +668,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -765,7 +774,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -907,7 +916,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -917,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433A841-7153-44ED-9730-8ADB27239D68}">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,21 +2010,295 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F4518F-E053-4336-B711-7AA8B14FF1BD}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E26D657-ECD6-4A33-97F0-8FDC9A60338F}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="B2">
+        <v>3.452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="B3">
+        <v>16.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.106</v>
+      </c>
+      <c r="B4">
+        <v>26.466000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="B5">
+        <v>37.972999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.129</v>
+      </c>
+      <c r="B6">
+        <v>47.177999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B7">
+        <v>54.082000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.155</v>
+      </c>
+      <c r="B8">
+        <v>60.985999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="B9">
+        <v>65.588999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.182</v>
+      </c>
+      <c r="B10">
+        <v>70.191999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="B11">
+        <v>73.644000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.216</v>
+      </c>
+      <c r="B12">
+        <v>77.096000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="B13">
+        <v>79.397000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.254</v>
+      </c>
+      <c r="B14">
+        <v>80.548000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="B15">
+        <v>81.698999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="B16">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.314</v>
+      </c>
+      <c r="B17">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="B18">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="B19">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="B20">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.443</v>
+      </c>
+      <c r="B21">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="B22">
+        <v>81.698999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="B23">
+        <v>81.698999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="B24">
+        <v>80.548000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.64</v>
+      </c>
+      <c r="B25">
+        <v>79.397000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="B26">
+        <v>78.247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="B27">
+        <v>77.096000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="B28">
+        <v>75.944999999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="B29">
+        <v>74.795000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="B30">
+        <v>73.644000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="B31">
+        <v>72.492999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="B32">
+        <v>71.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F4518F-E053-4336-B711-7AA8B14FF1BD}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2023,39 +2306,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{AD99E662-036F-455C-AF04-EDB24A6A27C0}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{44BBE0FB-15C6-4672-BA57-AA13C35E9C0F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{89108E00-8988-40E5-8BC6-D008EE3AF868}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2A6BC0BB735E644BCE53E48F728C05B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="068fbba309a89f3fc737bcec880766ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7cb7a32c-79a0-460d-898f-20ffd5321b11" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e6ab272ff8bfdb253a213921207b648" ns3:_="">
     <xsd:import namespace="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
@@ -2181,31 +2464,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{559E98B7-DD2C-4A6B-AA12-767DDCAB657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2221,4 +2495,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lucia's update: added SOEC
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
@@ -1,22 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luc.eco\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D04F7D4A-5AA1-49C7-B56F-B175AF9AC679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{D04F7D4A-5AA1-49C7-B56F-B175AF9AC679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{409DEA47-C896-4B0C-B397-6084BBA6B16C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-11505" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency_PEM" sheetId="5" r:id="rId1"/>
     <sheet name="Efficiency_Alkaline" sheetId="6" r:id="rId2"/>
-    <sheet name="Sources" sheetId="2" r:id="rId3"/>
+    <sheet name="Efficiency_SOEC" sheetId="7" r:id="rId3"/>
+    <sheet name="Sources" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="IQ_CH">110000</definedName>
+    <definedName name="IQ_CQ">5000</definedName>
+    <definedName name="IQ_CY">10000</definedName>
+    <definedName name="IQ_DAILY">500000</definedName>
+    <definedName name="IQ_DNTM" hidden="1">700000</definedName>
+    <definedName name="IQ_FH">100000</definedName>
+    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
+    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
+    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
+    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
+    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
+    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
+    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
+    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
+    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
+    <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
+    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
+    <definedName name="IQ_LTM">2000</definedName>
+    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
+    <definedName name="IQ_MONTH">15000</definedName>
+    <definedName name="IQ_MTD" hidden="1">800000</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">45429.7589699074</definedName>
+    <definedName name="IQ_NTM">6000</definedName>
+    <definedName name="IQ_QTD" hidden="1">750000</definedName>
+    <definedName name="IQ_TODAY" hidden="1">0</definedName>
+    <definedName name="IQ_WEEK">50000</definedName>
+    <definedName name="IQ_YTD">3000</definedName>
+    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Power [%]</t>
   </si>
@@ -57,12 +90,24 @@
   <si>
     <t>Sources</t>
   </si>
+  <si>
+    <t xml:space="preserve">SOEC: </t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9025002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and for the max efficiency: </t>
+  </si>
+  <si>
+    <t>https://www.sunfire.de/files/sunfire/images/content/Produkte_Technologie/factsheets/Sunfire-Factsheet-HyLink-SOEC_2023Nov.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +246,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,11 +601,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -619,9 +672,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -659,7 +712,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -765,7 +818,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -907,7 +960,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -917,13 +970,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433A841-7153-44ED-9730-8ADB27239D68}">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.05</v>
       </c>
@@ -939,7 +992,7 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.06</v>
       </c>
@@ -947,7 +1000,7 @@
         <v>0.70166666666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -955,7 +1008,7 @@
         <v>0.69142857142857139</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.08</v>
       </c>
@@ -963,7 +1016,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.09</v>
       </c>
@@ -971,7 +1024,7 @@
         <v>0.66111111111111109</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.1</v>
       </c>
@@ -979,7 +1032,7 @@
         <v>0.64500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.11</v>
       </c>
@@ -987,7 +1040,7 @@
         <v>0.63181818181818183</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.12</v>
       </c>
@@ -995,7 +1048,7 @@
         <v>0.62083333333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.13</v>
       </c>
@@ -1003,7 +1056,7 @@
         <v>0.61153846153846159</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.14000000000000001</v>
       </c>
@@ -1011,7 +1064,7 @@
         <v>0.60357142857142854</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.15</v>
       </c>
@@ -1019,7 +1072,7 @@
         <v>0.59733333333333338</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.16</v>
       </c>
@@ -1027,7 +1080,7 @@
         <v>0.59875</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.17</v>
       </c>
@@ -1035,7 +1088,7 @@
         <v>0.60058823529411764</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.18</v>
       </c>
@@ -1043,7 +1096,7 @@
         <v>0.60111111111111115</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.19</v>
       </c>
@@ -1051,7 +1104,7 @@
         <v>0.59578947368421054</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.2</v>
       </c>
@@ -1059,7 +1112,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.21</v>
       </c>
@@ -1067,7 +1120,7 @@
         <v>0.58666666666666667</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.22</v>
       </c>
@@ -1075,7 +1128,7 @@
         <v>0.58636363636363642</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.23</v>
       </c>
@@ -1083,7 +1136,7 @@
         <v>0.58782608695652172</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.24</v>
       </c>
@@ -1091,7 +1144,7 @@
         <v>0.58958333333333335</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.25</v>
       </c>
@@ -1099,7 +1152,7 @@
         <v>0.58760000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.26</v>
       </c>
@@ -1107,7 +1160,7 @@
         <v>0.58423076923076922</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.27</v>
       </c>
@@ -1115,7 +1168,7 @@
         <v>0.58111111111111113</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.28000000000000003</v>
       </c>
@@ -1123,7 +1176,7 @@
         <v>0.57892857142857146</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.28999999999999998</v>
       </c>
@@ -1131,7 +1184,7 @@
         <v>0.58068965517241378</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.3</v>
       </c>
@@ -1139,7 +1192,7 @@
         <v>0.58200000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.31</v>
       </c>
@@ -1147,7 +1200,7 @@
         <v>0.58225806451612905</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.32</v>
       </c>
@@ -1155,7 +1208,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.33</v>
       </c>
@@ -1163,7 +1216,7 @@
         <v>0.57757575757575752</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.34</v>
       </c>
@@ -1171,7 +1224,7 @@
         <v>0.57529411764705873</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.35</v>
       </c>
@@ -1179,7 +1232,7 @@
         <v>0.57571428571428562</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.36</v>
       </c>
@@ -1187,7 +1240,7 @@
         <v>0.5772222222222223</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.37</v>
       </c>
@@ -1195,7 +1248,7 @@
         <v>0.57837837837837835</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.38</v>
       </c>
@@ -1203,7 +1256,7 @@
         <v>0.57973684210526322</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.39</v>
       </c>
@@ -1211,7 +1264,7 @@
         <v>0.58102564102564103</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.4</v>
       </c>
@@ -1219,7 +1272,7 @@
         <v>0.58200000000000007</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.41</v>
       </c>
@@ -1227,7 +1280,7 @@
         <v>0.58317073170731704</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.42</v>
       </c>
@@ -1235,7 +1288,7 @@
         <v>0.5842857142857143</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.43</v>
       </c>
@@ -1243,7 +1296,7 @@
         <v>0.58511627906976749</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.44</v>
       </c>
@@ -1251,7 +1304,7 @@
         <v>0.58613636363636357</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.45</v>
       </c>
@@ -1259,7 +1312,7 @@
         <v>0.58911111111111114</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.46</v>
       </c>
@@ -1267,7 +1320,7 @@
         <v>0.592608695652174</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.47</v>
       </c>
@@ -1275,7 +1328,7 @@
         <v>0.5959574468085107</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.48</v>
       </c>
@@ -1283,7 +1336,7 @@
         <v>0.59895833333333337</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.49</v>
       </c>
@@ -1291,7 +1344,7 @@
         <v>0.59938775510204079</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.5</v>
       </c>
@@ -1299,7 +1352,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.51</v>
       </c>
@@ -1307,7 +1360,7 @@
         <v>0.5998039215686275</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.52</v>
       </c>
@@ -1315,7 +1368,7 @@
         <v>0.59788461538461535</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.53</v>
       </c>
@@ -1323,7 +1376,7 @@
         <v>0.59603773584905662</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.54</v>
       </c>
@@ -1331,7 +1384,7 @@
         <v>0.59444444444444444</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.55000000000000004</v>
       </c>
@@ -1339,7 +1392,7 @@
         <v>0.59272727272727277</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.56000000000000005</v>
       </c>
@@ -1347,7 +1400,7 @@
         <v>0.59107142857142858</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.56999999999999995</v>
       </c>
@@ -1355,7 +1408,7 @@
         <v>0.58947368421052637</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.57999999999999996</v>
       </c>
@@ -1363,7 +1416,7 @@
         <v>0.58793103448275863</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0.59</v>
       </c>
@@ -1371,7 +1424,7 @@
         <v>0.58644067796610166</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.6</v>
       </c>
@@ -1379,7 +1432,7 @@
         <v>0.58500000000000008</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>0.61</v>
       </c>
@@ -1387,7 +1440,7 @@
         <v>0.58377049180327867</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>0.62</v>
       </c>
@@ -1395,7 +1448,7 @@
         <v>0.58467741935483875</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>0.63</v>
       </c>
@@ -1403,7 +1456,7 @@
         <v>0.58730158730158732</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>0.64</v>
       </c>
@@ -1411,7 +1464,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0.65</v>
       </c>
@@ -1419,7 +1472,7 @@
         <v>0.59246153846153848</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>0.66</v>
       </c>
@@ -1427,7 +1480,7 @@
         <v>0.59106060606060606</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>0.67</v>
       </c>
@@ -1435,7 +1488,7 @@
         <v>0.58970149253731341</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>0.68</v>
       </c>
@@ -1443,7 +1496,7 @@
         <v>0.58838235294117647</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>0.69</v>
       </c>
@@ -1451,7 +1504,7 @@
         <v>0.58710144927536234</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>0.7</v>
       </c>
@@ -1459,7 +1512,7 @@
         <v>0.58585714285714285</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>0.71</v>
       </c>
@@ -1467,7 +1520,7 @@
         <v>0.58478873239436624</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>0.72</v>
       </c>
@@ -1475,7 +1528,7 @@
         <v>0.58361111111111119</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>0.73</v>
       </c>
@@ -1483,7 +1536,7 @@
         <v>0.58287671232876703</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0.74</v>
       </c>
@@ -1491,7 +1544,7 @@
         <v>0.58229729729729729</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>0.75</v>
       </c>
@@ -1499,7 +1552,7 @@
         <v>0.58160000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>0.76</v>
       </c>
@@ -1507,7 +1560,7 @@
         <v>0.58105263157894738</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>0.77</v>
       </c>
@@ -1515,7 +1568,7 @@
         <v>0.58051948051948055</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>0.78</v>
       </c>
@@ -1523,7 +1576,7 @@
         <v>0.58089743589743592</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>0.79</v>
       </c>
@@ -1531,7 +1584,7 @@
         <v>0.5815189873417721</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>0.8</v>
       </c>
@@ -1539,7 +1592,7 @@
         <v>0.582125</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>0.81</v>
       </c>
@@ -1547,7 +1600,7 @@
         <v>0.58259259259259255</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>0.82</v>
       </c>
@@ -1555,7 +1608,7 @@
         <v>0.58317073170731704</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>0.83</v>
       </c>
@@ -1563,7 +1616,7 @@
         <v>0.5834939759036144</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>0.84</v>
       </c>
@@ -1571,7 +1624,7 @@
         <v>0.58250000000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>0.85</v>
       </c>
@@ -1579,7 +1632,7 @@
         <v>0.58152941176470585</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.86</v>
       </c>
@@ -1587,7 +1640,7 @@
         <v>0.58058139534883724</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>0.87</v>
       </c>
@@ -1595,7 +1648,7 @@
         <v>0.5805747126436781</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>0.88</v>
       </c>
@@ -1603,7 +1656,7 @@
         <v>0.5810227272727273</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>0.89</v>
       </c>
@@ -1611,7 +1664,7 @@
         <v>0.58157303370786517</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>0.9</v>
       </c>
@@ -1619,7 +1672,7 @@
         <v>0.58111111111111113</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>0.91</v>
       </c>
@@ -1627,7 +1680,7 @@
         <v>0.58021978021978016</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>0.92</v>
       </c>
@@ -1635,7 +1688,7 @@
         <v>0.57934782608695645</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>0.93</v>
       </c>
@@ -1643,7 +1696,7 @@
         <v>0.57849462365591398</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>0.94</v>
       </c>
@@ -1651,7 +1704,7 @@
         <v>0.57765957446808502</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>0.95</v>
       </c>
@@ -1659,7 +1712,7 @@
         <v>0.57694736842105265</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>0.96</v>
       </c>
@@ -1667,7 +1720,7 @@
         <v>0.57614583333333336</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>0.97</v>
       </c>
@@ -1675,7 +1728,7 @@
         <v>0.57536082474226802</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>0.98</v>
       </c>
@@ -1683,7 +1736,7 @@
         <v>0.57459183673469394</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>0.99</v>
       </c>
@@ -1705,9 +1758,9 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1723,7 +1776,7 @@
         <v>0.61993799999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5.1989999999999996E-3</v>
       </c>
@@ -1731,7 +1784,7 @@
         <v>0.62460419999999983</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.2796999999999999E-2</v>
       </c>
@@ -1739,7 +1792,7 @@
         <v>0.62893710000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.0596E-2</v>
       </c>
@@ -1747,7 +1800,7 @@
         <v>0.63360329999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.8194E-2</v>
       </c>
@@ -1755,7 +1808,7 @@
         <v>0.63760289999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3.5992999999999997E-2</v>
       </c>
@@ -1763,7 +1816,7 @@
         <v>0.64193579999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4.879E-2</v>
       </c>
@@ -1771,7 +1824,7 @@
         <v>0.64626869999999992</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6.4186999999999994E-2</v>
       </c>
@@ -1779,7 +1832,7 @@
         <v>0.6506016</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8.3382999999999999E-2</v>
       </c>
@@ -1787,7 +1840,7 @@
         <v>0.65460119999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.103979</v>
       </c>
@@ -1795,7 +1848,7 @@
         <v>0.65726759999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.130774</v>
       </c>
@@ -1803,7 +1856,7 @@
         <v>0.65926739999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.15396899999999999</v>
       </c>
@@ -1811,7 +1864,7 @@
         <v>0.65926739999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.18216399999999999</v>
       </c>
@@ -1819,7 +1872,7 @@
         <v>0.65893409999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.21035799999999999</v>
       </c>
@@ -1827,7 +1880,7 @@
         <v>0.65760090000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.244951</v>
       </c>
@@ -1835,7 +1888,7 @@
         <v>0.65560109999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.278144</v>
       </c>
@@ -1843,7 +1896,7 @@
         <v>0.65260139999999989</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.314137</v>
       </c>
@@ -1851,7 +1904,7 @@
         <v>0.64960169999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.34233200000000003</v>
       </c>
@@ -1859,7 +1912,7 @@
         <v>0.64660200000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.37832399999999999</v>
       </c>
@@ -1867,7 +1920,7 @@
         <v>0.64326899999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.408918</v>
       </c>
@@ -1875,7 +1928,7 @@
         <v>0.63993599999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.441112</v>
       </c>
@@ -1883,7 +1936,7 @@
         <v>0.63660300000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.47190599999999999</v>
       </c>
@@ -1891,7 +1944,7 @@
         <v>0.63360329999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.50009999999999999</v>
       </c>
@@ -1899,7 +1952,7 @@
         <v>0.63060360000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.530694</v>
       </c>
@@ -1907,7 +1960,7 @@
         <v>0.62760389999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.56548699999999996</v>
       </c>
@@ -1915,7 +1968,7 @@
         <v>0.62393759999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.60647899999999999</v>
       </c>
@@ -1923,7 +1976,7 @@
         <v>0.61993799999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.64866999999999997</v>
       </c>
@@ -1931,7 +1984,7 @@
         <v>0.61560509999999991</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.689662</v>
       </c>
@@ -1939,7 +1992,7 @@
         <v>0.61193879999999989</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.73725300000000005</v>
       </c>
@@ -1947,7 +2000,7 @@
         <v>0.60727259999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.78724300000000003</v>
       </c>
@@ -1955,7 +2008,7 @@
         <v>0.60260639999999988</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.83583300000000005</v>
       </c>
@@ -1963,7 +2016,7 @@
         <v>0.59860679999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.88082400000000005</v>
       </c>
@@ -1971,7 +2024,7 @@
         <v>0.59460719999999989</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.92561499999999997</v>
       </c>
@@ -1979,7 +2032,7 @@
         <v>0.59094089999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.96020799999999995</v>
       </c>
@@ -1987,7 +2040,7 @@
         <v>0.58760789999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2001,21 +2054,292 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9CF4AA-6B39-4ABA-BF7A-FB938F21D187}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3.452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>16.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>0.106</v>
+      </c>
+      <c r="B4" s="4">
+        <v>26.466000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="B5" s="4">
+        <v>37.972999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>0.129</v>
+      </c>
+      <c r="B6" s="4">
+        <v>47.177999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B7" s="4">
+        <v>54.082000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>0.155</v>
+      </c>
+      <c r="B8" s="4">
+        <v>60.985999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="B9" s="4">
+        <v>65.588999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>0.182</v>
+      </c>
+      <c r="B10" s="4">
+        <v>70.191999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="B11" s="4">
+        <v>73.644000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>0.216</v>
+      </c>
+      <c r="B12" s="4">
+        <v>77.096000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="B13" s="4">
+        <v>79.397000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>0.254</v>
+      </c>
+      <c r="B14" s="4">
+        <v>80.548000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="B15" s="4">
+        <v>81.698999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="B16" s="4">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>0.314</v>
+      </c>
+      <c r="B17" s="4">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="B18" s="4">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="B19" s="4">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="B20" s="4">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>0.443</v>
+      </c>
+      <c r="B21" s="4">
+        <v>82.849000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="B22" s="4">
+        <v>81.698999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="B23" s="4">
+        <v>81.698999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="B24" s="4">
+        <v>80.548000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="B25" s="4">
+        <v>79.397000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="B26" s="4">
+        <v>78.247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="B27" s="4">
+        <v>77.096000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="B28" s="4">
+        <v>75.944999999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="B29" s="4">
+        <v>74.795000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="B30" s="4">
+        <v>73.644000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="B31" s="4">
+        <v>72.492999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="B32" s="4">
+        <v>71.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F4518F-E053-4336-B711-7AA8B14FF1BD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2023,39 +2347,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{AD99E662-036F-455C-AF04-EDB24A6A27C0}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{44BBE0FB-15C6-4672-BA57-AA13C35E9C0F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C22FC715-A4F9-4404-BD43-3AFD61FE2E30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2A6BC0BB735E644BCE53E48F728C05B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="068fbba309a89f3fc737bcec880766ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7cb7a32c-79a0-460d-898f-20ffd5321b11" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e6ab272ff8bfdb253a213921207b648" ns3:_="">
     <xsd:import namespace="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
@@ -2181,31 +2510,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{559E98B7-DD2C-4A6B-AA12-767DDCAB657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2221,4 +2541,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed bug in electrolyzer table + improved adjustment method for Alkaline + SOEC
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{D04F7D4A-5AA1-49C7-B56F-B175AF9AC679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{409DEA47-C896-4B0C-B397-6084BBA6B16C}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{D04F7D4A-5AA1-49C7-B56F-B175AF9AC679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF39A0AA-80F4-468D-BF07-96CB425DBA6C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-11505" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency_PEM" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Sources" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="CIQWBGuid" hidden="1">"9dba8f33-1087-4509-8f71-f29d917cc8e9"</definedName>
+    <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -665,10 +667,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -971,7 +969,7 @@
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2058,7 +2056,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,248 +2073,248 @@
       <c r="A2" s="4">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="B2" s="4">
-        <v>3.452</v>
+      <c r="B2" s="1">
+        <v>3.4520000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="B3" s="4">
-        <v>16.11</v>
+      <c r="B3" s="1">
+        <v>0.16109999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>0.106</v>
       </c>
-      <c r="B4" s="4">
-        <v>26.466000000000001</v>
+      <c r="B4" s="1">
+        <v>0.26466000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>0.11700000000000001</v>
       </c>
-      <c r="B5" s="4">
-        <v>37.972999999999999</v>
+      <c r="B5" s="1">
+        <v>0.37973000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>0.129</v>
       </c>
-      <c r="B6" s="4">
-        <v>47.177999999999997</v>
+      <c r="B6" s="1">
+        <v>0.47177999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="B7" s="4">
-        <v>54.082000000000001</v>
+      <c r="B7" s="1">
+        <v>0.54081999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>0.155</v>
       </c>
-      <c r="B8" s="4">
-        <v>60.985999999999997</v>
+      <c r="B8" s="1">
+        <v>0.60985999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>0.16700000000000001</v>
       </c>
-      <c r="B9" s="4">
-        <v>65.588999999999999</v>
+      <c r="B9" s="1">
+        <v>0.65588999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>0.182</v>
       </c>
-      <c r="B10" s="4">
-        <v>70.191999999999993</v>
+      <c r="B10" s="1">
+        <v>0.70191999999999988</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>0.19700000000000001</v>
       </c>
-      <c r="B11" s="4">
-        <v>73.644000000000005</v>
+      <c r="B11" s="1">
+        <v>0.73644000000000009</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>0.216</v>
       </c>
-      <c r="B12" s="4">
-        <v>77.096000000000004</v>
+      <c r="B12" s="1">
+        <v>0.77096000000000009</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>0.23499999999999999</v>
       </c>
-      <c r="B13" s="4">
-        <v>79.397000000000006</v>
+      <c r="B13" s="1">
+        <v>0.79397000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>0.254</v>
       </c>
-      <c r="B14" s="4">
-        <v>80.548000000000002</v>
+      <c r="B14" s="1">
+        <v>0.80547999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>0.27300000000000002</v>
       </c>
-      <c r="B15" s="4">
-        <v>81.698999999999998</v>
+      <c r="B15" s="1">
+        <v>0.81698999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>0.29199999999999998</v>
       </c>
-      <c r="B16" s="4">
-        <v>82.849000000000004</v>
+      <c r="B16" s="1">
+        <v>0.82849000000000006</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>0.314</v>
       </c>
-      <c r="B17" s="4">
-        <v>82.849000000000004</v>
+      <c r="B17" s="1">
+        <v>0.82849000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>0.34100000000000003</v>
       </c>
-      <c r="B18" s="4">
-        <v>82.849000000000004</v>
+      <c r="B18" s="1">
+        <v>0.82849000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>0.36699999999999999</v>
       </c>
-      <c r="B19" s="4">
-        <v>82.849000000000004</v>
+      <c r="B19" s="1">
+        <v>0.82849000000000006</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>0.39800000000000002</v>
       </c>
-      <c r="B20" s="4">
-        <v>82.849000000000004</v>
+      <c r="B20" s="1">
+        <v>0.82849000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>0.443</v>
       </c>
-      <c r="B21" s="4">
-        <v>82.849000000000004</v>
+      <c r="B21" s="1">
+        <v>0.82849000000000006</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>0.48899999999999999</v>
       </c>
-      <c r="B22" s="4">
-        <v>81.698999999999998</v>
+      <c r="B22" s="1">
+        <v>0.81698999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>0.54200000000000004</v>
       </c>
-      <c r="B23" s="4">
-        <v>81.698999999999998</v>
+      <c r="B23" s="1">
+        <v>0.81698999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>0.58699999999999997</v>
       </c>
-      <c r="B24" s="4">
-        <v>80.548000000000002</v>
+      <c r="B24" s="1">
+        <v>0.80547999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>0.64</v>
       </c>
-      <c r="B25" s="4">
-        <v>79.397000000000006</v>
+      <c r="B25" s="1">
+        <v>0.79397000000000006</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>0.70799999999999996</v>
       </c>
-      <c r="B26" s="4">
-        <v>78.247</v>
+      <c r="B26" s="1">
+        <v>0.78247</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>0.76500000000000001</v>
       </c>
-      <c r="B27" s="4">
-        <v>77.096000000000004</v>
+      <c r="B27" s="1">
+        <v>0.77096000000000009</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>0.81799999999999995</v>
       </c>
-      <c r="B28" s="4">
-        <v>75.944999999999993</v>
+      <c r="B28" s="1">
+        <v>0.75944999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>0.86699999999999999</v>
       </c>
-      <c r="B29" s="4">
-        <v>74.795000000000002</v>
+      <c r="B29" s="1">
+        <v>0.74795</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>0.92400000000000004</v>
       </c>
-      <c r="B30" s="4">
-        <v>73.644000000000005</v>
+      <c r="B30" s="1">
+        <v>0.73644000000000009</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>0.96199999999999997</v>
       </c>
-      <c r="B31" s="4">
-        <v>72.492999999999995</v>
+      <c r="B31" s="1">
+        <v>0.72492999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>0.99099999999999999</v>
       </c>
-      <c r="B32" s="4">
-        <v>71.5</v>
+      <c r="B32" s="1">
+        <v>0.71499999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2385,6 +2383,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2A6BC0BB735E644BCE53E48F728C05B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="068fbba309a89f3fc737bcec880766ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7cb7a32c-79a0-460d-898f-20ffd5321b11" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e6ab272ff8bfdb253a213921207b648" ns3:_="">
     <xsd:import namespace="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
@@ -2510,22 +2523,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{559E98B7-DD2C-4A6B-AA12-767DDCAB657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2541,28 +2563,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7cb7a32c-79a0-460d-898f-20ffd5321b11"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
hot fix for pem efficiency
the current curve is not strictly monotonically decreasing after max efficiency point. This is causing problems with the operating points efficiency calculation.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{D04F7D4A-5AA1-49C7-B56F-B175AF9AC679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF39A0AA-80F4-468D-BF07-96CB425DBA6C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9A7EF3-3C5A-4FC5-9102-093E5F530029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency_PEM" sheetId="5" r:id="rId1"/>
@@ -966,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433A841-7153-44ED-9730-8ADB27239D68}">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,763 +984,473 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>0.71599999999999997</v>
+        <v>0.61993799999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>0.06</v>
+        <v>5.1989999999999996E-3</v>
       </c>
       <c r="B3" s="2">
-        <v>0.70166666666666666</v>
+        <v>0.62460419999999983</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>7.0000000000000007E-2</v>
+        <v>1.2796999999999999E-2</v>
       </c>
       <c r="B4" s="2">
-        <v>0.69142857142857139</v>
+        <v>0.62893710000000003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>0.08</v>
+        <v>2.0596E-2</v>
       </c>
       <c r="B5" s="2">
-        <v>0.68</v>
+        <v>0.63360329999999998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>0.09</v>
+        <v>2.8194E-2</v>
       </c>
       <c r="B6" s="2">
-        <v>0.66111111111111109</v>
+        <v>0.63760289999999997</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>0.1</v>
+        <v>3.5992999999999997E-2</v>
       </c>
       <c r="B7" s="2">
-        <v>0.64500000000000002</v>
+        <v>0.64193579999999995</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0.11</v>
+        <v>4.879E-2</v>
       </c>
       <c r="B8" s="2">
-        <v>0.63181818181818183</v>
+        <v>0.64626869999999992</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0.12</v>
+        <v>6.4186999999999994E-2</v>
       </c>
       <c r="B9" s="2">
-        <v>0.62083333333333335</v>
+        <v>0.6506016</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>0.13</v>
+        <v>8.3382999999999999E-2</v>
       </c>
       <c r="B10" s="2">
-        <v>0.61153846153846159</v>
+        <v>0.65460119999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0.14000000000000001</v>
+        <v>0.103979</v>
       </c>
       <c r="B11" s="2">
-        <v>0.60357142857142854</v>
+        <v>0.65726759999999995</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0.15</v>
+        <v>0.130774</v>
       </c>
       <c r="B12" s="2">
-        <v>0.59733333333333338</v>
+        <v>0.65926739999999995</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0.16</v>
+        <v>0.15396899999999999</v>
       </c>
       <c r="B13" s="2">
-        <v>0.59875</v>
+        <v>0.65926739999999995</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0.17</v>
+        <v>0.18216399999999999</v>
       </c>
       <c r="B14" s="2">
-        <v>0.60058823529411764</v>
+        <v>0.65893409999999997</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0.18</v>
+        <v>0.21035799999999999</v>
       </c>
       <c r="B15" s="2">
-        <v>0.60111111111111115</v>
+        <v>0.65760090000000004</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>0.19</v>
+        <v>0.244951</v>
       </c>
       <c r="B16" s="2">
-        <v>0.59578947368421054</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.65560109999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>0.2</v>
+        <v>0.278144</v>
       </c>
       <c r="B17" s="2">
-        <v>0.59099999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.65260139999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>0.21</v>
+        <v>0.314137</v>
       </c>
       <c r="B18" s="2">
-        <v>0.58666666666666667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.64960169999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>0.22</v>
+        <v>0.34233200000000003</v>
       </c>
       <c r="B19" s="2">
-        <v>0.58636363636363642</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.64660200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>0.23</v>
+        <v>0.37832399999999999</v>
       </c>
       <c r="B20" s="2">
-        <v>0.58782608695652172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.64326899999999998</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>0.24</v>
+        <v>0.408918</v>
       </c>
       <c r="B21" s="2">
-        <v>0.58958333333333335</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.63993599999999995</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>0.25</v>
+        <v>0.441112</v>
       </c>
       <c r="B22" s="2">
-        <v>0.58760000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.63660300000000003</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>0.26</v>
+        <v>0.47190599999999999</v>
       </c>
       <c r="B23" s="2">
-        <v>0.58423076923076922</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.63360329999999998</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>0.27</v>
+        <v>0.50009999999999999</v>
       </c>
       <c r="B24" s="2">
-        <v>0.58111111111111113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.63060360000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>0.28000000000000003</v>
+        <v>0.530694</v>
       </c>
       <c r="B25" s="2">
-        <v>0.57892857142857146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.62760389999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>0.28999999999999998</v>
+        <v>0.56548699999999996</v>
       </c>
       <c r="B26" s="2">
-        <v>0.58068965517241378</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.62393759999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>0.3</v>
+        <v>0.60647899999999999</v>
       </c>
       <c r="B27" s="2">
-        <v>0.58200000000000007</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.61993799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>0.31</v>
+        <v>0.64866999999999997</v>
       </c>
       <c r="B28" s="2">
-        <v>0.58225806451612905</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.61560509999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>0.32</v>
+        <v>0.689662</v>
       </c>
       <c r="B29" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.61193879999999989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>0.33</v>
+        <v>0.73725300000000005</v>
       </c>
       <c r="B30" s="2">
-        <v>0.57757575757575752</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.60727259999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>0.34</v>
+        <v>0.78724300000000003</v>
       </c>
       <c r="B31" s="2">
-        <v>0.57529411764705873</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.60260639999999988</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>0.35</v>
+        <v>0.83583300000000005</v>
       </c>
       <c r="B32" s="2">
-        <v>0.57571428571428562</v>
+        <v>0.59860679999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>0.36</v>
+        <v>0.88082400000000005</v>
       </c>
       <c r="B33" s="2">
-        <v>0.5772222222222223</v>
+        <v>0.59460719999999989</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>0.37</v>
+        <v>0.92561499999999997</v>
       </c>
       <c r="B34" s="2">
-        <v>0.57837837837837835</v>
+        <v>0.59094089999999999</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>0.38</v>
+        <v>0.96020799999999995</v>
       </c>
       <c r="B35" s="2">
-        <v>0.57973684210526322</v>
+        <v>0.58760789999999996</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>0.39</v>
+        <v>1</v>
       </c>
       <c r="B36" s="2">
-        <v>0.58102564102564103</v>
+        <v>0.5849415</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>0.4</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0.58200000000000007</v>
-      </c>
+      <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>0.41</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0.58317073170731704</v>
-      </c>
+      <c r="B38" s="1"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>0.42</v>
-      </c>
-      <c r="B39" s="1">
-        <v>0.5842857142857143</v>
-      </c>
+      <c r="B39" s="1"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>0.43</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0.58511627906976749</v>
-      </c>
+      <c r="B40" s="1"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>0.44</v>
-      </c>
-      <c r="B41" s="1">
-        <v>0.58613636363636357</v>
-      </c>
+      <c r="B41" s="1"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>0.45</v>
-      </c>
-      <c r="B42" s="1">
-        <v>0.58911111111111114</v>
-      </c>
+      <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>0.46</v>
-      </c>
-      <c r="B43" s="1">
-        <v>0.592608695652174</v>
-      </c>
+      <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>0.47</v>
-      </c>
-      <c r="B44" s="1">
-        <v>0.5959574468085107</v>
-      </c>
+      <c r="B44" s="1"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>0.48</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0.59895833333333337</v>
-      </c>
+      <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>0.49</v>
-      </c>
-      <c r="B46" s="1">
-        <v>0.59938775510204079</v>
-      </c>
+      <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>0.5</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0.6</v>
-      </c>
+      <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>0.51</v>
-      </c>
-      <c r="B48" s="1">
-        <v>0.5998039215686275</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>0.52</v>
-      </c>
-      <c r="B49" s="1">
-        <v>0.59788461538461535</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>0.53</v>
-      </c>
-      <c r="B50" s="1">
-        <v>0.59603773584905662</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>0.54</v>
-      </c>
-      <c r="B51" s="1">
-        <v>0.59444444444444444</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="B52" s="1">
-        <v>0.59272727272727277</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="B53" s="1">
-        <v>0.59107142857142858</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="B54" s="1">
-        <v>0.58947368421052637</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0.58793103448275863</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>0.59</v>
-      </c>
-      <c r="B56" s="1">
-        <v>0.58644067796610166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>0.6</v>
-      </c>
-      <c r="B57" s="1">
-        <v>0.58500000000000008</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>0.61</v>
-      </c>
-      <c r="B58" s="1">
-        <v>0.58377049180327867</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>0.62</v>
-      </c>
-      <c r="B59" s="1">
-        <v>0.58467741935483875</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>0.63</v>
-      </c>
-      <c r="B60" s="1">
-        <v>0.58730158730158732</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>0.64</v>
-      </c>
-      <c r="B61" s="1">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>0.65</v>
-      </c>
-      <c r="B62" s="1">
-        <v>0.59246153846153848</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>0.66</v>
-      </c>
-      <c r="B63" s="1">
-        <v>0.59106060606060606</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>0.67</v>
-      </c>
-      <c r="B64" s="1">
-        <v>0.58970149253731341</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>0.68</v>
-      </c>
-      <c r="B65" s="1">
-        <v>0.58838235294117647</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>0.69</v>
-      </c>
-      <c r="B66" s="1">
-        <v>0.58710144927536234</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>0.7</v>
-      </c>
-      <c r="B67" s="1">
-        <v>0.58585714285714285</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>0.71</v>
-      </c>
-      <c r="B68" s="1">
-        <v>0.58478873239436624</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>0.72</v>
-      </c>
-      <c r="B69" s="1">
-        <v>0.58361111111111119</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>0.73</v>
-      </c>
-      <c r="B70" s="1">
-        <v>0.58287671232876703</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>0.74</v>
-      </c>
-      <c r="B71" s="1">
-        <v>0.58229729729729729</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>0.75</v>
-      </c>
-      <c r="B72" s="1">
-        <v>0.58160000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>0.76</v>
-      </c>
-      <c r="B73" s="1">
-        <v>0.58105263157894738</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>0.77</v>
-      </c>
-      <c r="B74" s="1">
-        <v>0.58051948051948055</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>0.78</v>
-      </c>
-      <c r="B75" s="1">
-        <v>0.58089743589743592</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>0.79</v>
-      </c>
-      <c r="B76" s="1">
-        <v>0.5815189873417721</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>0.8</v>
-      </c>
-      <c r="B77" s="1">
-        <v>0.582125</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>0.81</v>
-      </c>
-      <c r="B78" s="1">
-        <v>0.58259259259259255</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>0.82</v>
-      </c>
-      <c r="B79" s="1">
-        <v>0.58317073170731704</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>0.83</v>
-      </c>
-      <c r="B80" s="1">
-        <v>0.5834939759036144</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>0.84</v>
-      </c>
-      <c r="B81" s="1">
-        <v>0.58250000000000002</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>0.85</v>
-      </c>
-      <c r="B82" s="1">
-        <v>0.58152941176470585</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>0.86</v>
-      </c>
-      <c r="B83" s="1">
-        <v>0.58058139534883724</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>0.87</v>
-      </c>
-      <c r="B84" s="1">
-        <v>0.5805747126436781</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>0.88</v>
-      </c>
-      <c r="B85" s="1">
-        <v>0.5810227272727273</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <v>0.89</v>
-      </c>
-      <c r="B86" s="1">
-        <v>0.58157303370786517</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>0.9</v>
-      </c>
-      <c r="B87" s="1">
-        <v>0.58111111111111113</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>0.91</v>
-      </c>
-      <c r="B88" s="1">
-        <v>0.58021978021978016</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>0.92</v>
-      </c>
-      <c r="B89" s="1">
-        <v>0.57934782608695645</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>0.93</v>
-      </c>
-      <c r="B90" s="1">
-        <v>0.57849462365591398</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>0.94</v>
-      </c>
-      <c r="B91" s="1">
-        <v>0.57765957446808502</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>0.95</v>
-      </c>
-      <c r="B92" s="1">
-        <v>0.57694736842105265</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>0.96</v>
-      </c>
-      <c r="B93" s="1">
-        <v>0.57614583333333336</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>0.97</v>
-      </c>
-      <c r="B94" s="1">
-        <v>0.57536082474226802</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>0.98</v>
-      </c>
-      <c r="B95" s="1">
-        <v>0.57459183673469394</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>0.99</v>
-      </c>
-      <c r="B96" s="1">
-        <v>0.57383838383838381</v>
-      </c>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B98" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1752,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20040AC2-246C-4C76-A39F-5F3C71B48CC3}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2055,7 +1765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9CF4AA-6B39-4ABA-BF7A-FB938F21D187}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2327,7 +2037,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>